<commit_message>
fixed formDef.json files since they cannot have integers in the value list.
</commit_message>
<xml_diff>
--- a/app/tables/femaleClients/forms/client6Month/client6Month.xlsx
+++ b/app/tables/femaleClients/forms/client6Month/client6Month.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="31400" yWindow="1660" windowWidth="28800" windowHeight="16020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="31780" yWindow="1840" windowWidth="25600" windowHeight="16020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="337">
   <si>
     <t>type</t>
   </si>
@@ -975,13 +975,76 @@
   </si>
   <si>
     <t xml:space="preserve">Postpartum hemorrhage </t>
+  </si>
+  <si>
+    <t>a0</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>a5</t>
+  </si>
+  <si>
+    <t>a888</t>
+  </si>
+  <si>
+    <t>a666</t>
+  </si>
+  <si>
+    <t>a777</t>
+  </si>
+  <si>
+    <t>a999</t>
+  </si>
+  <si>
+    <t>a6</t>
+  </si>
+  <si>
+    <t>a7</t>
+  </si>
+  <si>
+    <t>a8</t>
+  </si>
+  <si>
+    <t>a9</t>
+  </si>
+  <si>
+    <t>a10</t>
+  </si>
+  <si>
+    <t>a11</t>
+  </si>
+  <si>
+    <t>a12</t>
+  </si>
+  <si>
+    <t>a13</t>
+  </si>
+  <si>
+    <t>a14</t>
+  </si>
+  <si>
+    <t>a15</t>
+  </si>
+  <si>
+    <t>a16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -999,6 +1062,22 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1042,9 +1121,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1088,7 +1171,11 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -2261,18 +2348,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C231"/>
+  <dimension ref="A1:D231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="A225" sqref="A225:XFD231"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="2"/>
     <col min="3" max="3" width="51.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="50.33203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="21.5" style="2"/>
   </cols>
   <sheetData>
@@ -2280,7 +2366,7 @@
       <c r="A1" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>293</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2291,8 +2377,8 @@
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="2">
-        <v>0</v>
+      <c r="B2" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>19</v>
@@ -2302,8 +2388,8 @@
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2">
-        <v>1</v>
+      <c r="B3" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -2313,8 +2399,8 @@
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="2">
-        <v>2</v>
+      <c r="B4" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>27</v>
@@ -2324,8 +2410,8 @@
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="2">
-        <v>3</v>
+      <c r="B5" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>28</v>
@@ -2335,8 +2421,8 @@
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
+      <c r="B6" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>29</v>
@@ -2346,8 +2432,8 @@
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="1">
-        <v>2</v>
+      <c r="B7" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
@@ -2357,8 +2443,8 @@
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="1">
-        <v>1</v>
+      <c r="B8" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2368,8 +2454,8 @@
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="1">
-        <v>2</v>
+      <c r="B9" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
@@ -2379,8 +2465,8 @@
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="1">
-        <v>3</v>
+      <c r="B10" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>34</v>
@@ -2390,8 +2476,8 @@
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="1">
-        <v>4</v>
+      <c r="B11" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>35</v>
@@ -2401,8 +2487,8 @@
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="1">
-        <v>5</v>
+      <c r="B12" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>37</v>
@@ -2412,8 +2498,8 @@
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="1">
-        <v>888</v>
+      <c r="B13" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>36</v>
@@ -2423,8 +2509,8 @@
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="2">
-        <v>1</v>
+      <c r="B14" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>15</v>
@@ -2434,8 +2520,8 @@
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="2">
-        <v>0</v>
+      <c r="B15" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>
@@ -2445,8 +2531,8 @@
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="1">
-        <v>888</v>
+      <c r="B16" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>36</v>
@@ -2456,8 +2542,8 @@
       <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="1">
-        <v>1</v>
+      <c r="B17" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
@@ -2467,8 +2553,8 @@
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="1">
-        <v>666</v>
+      <c r="B18" s="2" t="s">
+        <v>323</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>42</v>
@@ -2478,8 +2564,8 @@
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="1">
-        <v>777</v>
+      <c r="B19" s="2" t="s">
+        <v>324</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>43</v>
@@ -2489,8 +2575,8 @@
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="1">
-        <v>888</v>
+      <c r="B20" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>23</v>
@@ -2500,8 +2586,8 @@
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="1">
-        <v>999</v>
+      <c r="B21" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>22</v>
@@ -2511,8 +2597,8 @@
       <c r="A22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="2">
-        <v>0</v>
+      <c r="B22" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>19</v>
@@ -2522,8 +2608,8 @@
       <c r="A23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="2">
-        <v>1</v>
+      <c r="B23" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>20</v>
@@ -2533,8 +2619,8 @@
       <c r="A24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="2">
-        <v>2</v>
+      <c r="B24" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>44</v>
@@ -2544,8 +2630,8 @@
       <c r="A25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="2">
-        <v>888</v>
+      <c r="B25" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>23</v>
@@ -2555,8 +2641,8 @@
       <c r="A26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="1">
-        <v>999</v>
+      <c r="B26" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>22</v>
@@ -2566,8 +2652,8 @@
       <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
+      <c r="B27" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>15</v>
@@ -2577,8 +2663,8 @@
       <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="2">
-        <v>0</v>
+      <c r="B28" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>16</v>
@@ -2588,8 +2674,8 @@
       <c r="A29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="1">
-        <v>888</v>
+      <c r="B29" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>36</v>
@@ -2599,8 +2685,8 @@
       <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="1">
-        <v>999</v>
+      <c r="B30" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>22</v>
@@ -2610,8 +2696,8 @@
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="2">
-        <v>1</v>
+      <c r="B31" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>15</v>
@@ -2621,8 +2707,8 @@
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="2">
-        <v>0</v>
+      <c r="B32" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>16</v>
@@ -2632,8 +2718,8 @@
       <c r="A33" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="2">
-        <v>1</v>
+      <c r="B33" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>47</v>
@@ -2643,8 +2729,8 @@
       <c r="A34" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="2">
-        <v>2</v>
+      <c r="B34" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>48</v>
@@ -2654,8 +2740,8 @@
       <c r="A35" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="1">
-        <v>888</v>
+      <c r="B35" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>36</v>
@@ -2665,8 +2751,8 @@
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="1">
-        <v>999</v>
+      <c r="B36" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>22</v>
@@ -2676,8 +2762,8 @@
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="2">
-        <v>1</v>
+      <c r="B37" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>176</v>
@@ -2687,8 +2773,8 @@
       <c r="A38" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="2">
-        <v>0</v>
+      <c r="B38" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>51</v>
@@ -2698,8 +2784,8 @@
       <c r="A39" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="2">
-        <v>2</v>
+      <c r="B39" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>52</v>
@@ -2709,8 +2795,8 @@
       <c r="A40" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="1">
-        <v>888</v>
+      <c r="B40" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>36</v>
@@ -2720,8 +2806,8 @@
       <c r="A41" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="1">
-        <v>999</v>
+      <c r="B41" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>22</v>
@@ -2731,8 +2817,8 @@
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="1">
-        <v>1</v>
+      <c r="B42" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>54</v>
@@ -2742,8 +2828,8 @@
       <c r="A43" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="1">
-        <v>2</v>
+      <c r="B43" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>55</v>
@@ -2753,8 +2839,8 @@
       <c r="A44" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="1">
-        <v>3</v>
+      <c r="B44" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>56</v>
@@ -2764,8 +2850,8 @@
       <c r="A45" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="1">
-        <v>4</v>
+      <c r="B45" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>21</v>
@@ -2775,8 +2861,8 @@
       <c r="A46" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="1">
-        <v>888</v>
+      <c r="B46" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>36</v>
@@ -2786,8 +2872,8 @@
       <c r="A47" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="1">
-        <v>999</v>
+      <c r="B47" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>22</v>
@@ -2797,8 +2883,8 @@
       <c r="A48" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="2">
-        <v>1</v>
+      <c r="B48" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>177</v>
@@ -2808,8 +2894,8 @@
       <c r="A49" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B49" s="2">
-        <v>0</v>
+      <c r="B49" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>58</v>
@@ -2819,8 +2905,8 @@
       <c r="A50" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="2">
-        <v>2</v>
+      <c r="B50" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>178</v>
@@ -2830,8 +2916,8 @@
       <c r="A51" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="1">
-        <v>888</v>
+      <c r="B51" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>36</v>
@@ -2841,8 +2927,8 @@
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="1">
-        <v>999</v>
+      <c r="B52" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>22</v>
@@ -2852,8 +2938,8 @@
       <c r="A53" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B53" s="1">
-        <v>1</v>
+      <c r="B53" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>60</v>
@@ -2863,8 +2949,8 @@
       <c r="A54" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="1">
-        <v>2</v>
+      <c r="B54" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>61</v>
@@ -2874,8 +2960,8 @@
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B55" s="1">
-        <v>3</v>
+      <c r="B55" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>62</v>
@@ -2885,8 +2971,8 @@
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="1">
-        <v>4</v>
+      <c r="B56" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>63</v>
@@ -2896,8 +2982,8 @@
       <c r="A57" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="1">
-        <v>5</v>
+      <c r="B57" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>64</v>
@@ -2907,8 +2993,8 @@
       <c r="A58" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="1">
-        <v>6</v>
+      <c r="B58" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>65</v>
@@ -2918,8 +3004,8 @@
       <c r="A59" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="1">
-        <v>7</v>
+      <c r="B59" s="2" t="s">
+        <v>327</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>37</v>
@@ -2929,8 +3015,8 @@
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="1">
-        <v>888</v>
+      <c r="B60" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>66</v>
@@ -2940,8 +3026,8 @@
       <c r="A61" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B61" s="1">
-        <v>1</v>
+      <c r="B61" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>60</v>
@@ -2951,8 +3037,8 @@
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B62" s="1">
-        <v>2</v>
+      <c r="B62" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>61</v>
@@ -2962,8 +3048,8 @@
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="1">
-        <v>3</v>
+      <c r="B63" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>62</v>
@@ -2973,8 +3059,8 @@
       <c r="A64" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="1">
-        <v>4</v>
+      <c r="B64" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>63</v>
@@ -2984,8 +3070,8 @@
       <c r="A65" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B65" s="1">
-        <v>5</v>
+      <c r="B65" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>64</v>
@@ -2995,8 +3081,8 @@
       <c r="A66" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B66" s="1">
-        <v>6</v>
+      <c r="B66" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>65</v>
@@ -3006,8 +3092,8 @@
       <c r="A67" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="1">
-        <v>7</v>
+      <c r="B67" s="2" t="s">
+        <v>327</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>37</v>
@@ -3017,8 +3103,8 @@
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="1">
-        <v>8</v>
+      <c r="B68" s="2" t="s">
+        <v>328</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>68</v>
@@ -3028,8 +3114,8 @@
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B69" s="1">
-        <v>888</v>
+      <c r="B69" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>66</v>
@@ -3039,8 +3125,8 @@
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="2">
-        <v>1</v>
+      <c r="B70" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>15</v>
@@ -3050,8 +3136,8 @@
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B71" s="2">
-        <v>0</v>
+      <c r="B71" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>16</v>
@@ -3061,8 +3147,8 @@
       <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="1">
-        <v>666</v>
+      <c r="B72" s="2" t="s">
+        <v>323</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>70</v>
@@ -3072,8 +3158,8 @@
       <c r="A73" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="1">
-        <v>888</v>
+      <c r="B73" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>36</v>
@@ -3083,8 +3169,8 @@
       <c r="A74" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="1">
-        <v>999</v>
+      <c r="B74" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>22</v>
@@ -3094,7 +3180,7 @@
       <c r="A75" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="2" t="s">
         <v>168</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -3105,7 +3191,7 @@
       <c r="A76" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C76" s="2" t="s">
@@ -3116,7 +3202,7 @@
       <c r="A77" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C77" s="1" t="s">
@@ -3127,8 +3213,8 @@
       <c r="A78" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B78" s="1">
-        <v>888</v>
+      <c r="B78" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>36</v>
@@ -3138,8 +3224,8 @@
       <c r="A79" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B79" s="1">
-        <v>999</v>
+      <c r="B79" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>22</v>
@@ -3149,8 +3235,8 @@
       <c r="A80" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B80" s="1">
-        <v>1</v>
+      <c r="B80" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>74</v>
@@ -3160,8 +3246,8 @@
       <c r="A81" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B81" s="1">
-        <v>2</v>
+      <c r="B81" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>75</v>
@@ -3171,8 +3257,8 @@
       <c r="A82" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B82" s="1">
-        <v>3</v>
+      <c r="B82" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>76</v>
@@ -3182,8 +3268,8 @@
       <c r="A83" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B83" s="1">
-        <v>888</v>
+      <c r="B83" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>23</v>
@@ -3193,8 +3279,8 @@
       <c r="A84" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="1">
-        <v>999</v>
+      <c r="B84" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>22</v>
@@ -3204,8 +3290,8 @@
       <c r="A85" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B85" s="1">
-        <v>1</v>
+      <c r="B85" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>78</v>
@@ -3215,8 +3301,8 @@
       <c r="A86" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B86" s="1">
-        <v>2</v>
+      <c r="B86" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>79</v>
@@ -3226,8 +3312,8 @@
       <c r="A87" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B87" s="1">
-        <v>3</v>
+      <c r="B87" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>80</v>
@@ -3237,8 +3323,8 @@
       <c r="A88" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B88" s="1">
-        <v>4</v>
+      <c r="B88" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>81</v>
@@ -3248,8 +3334,8 @@
       <c r="A89" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B89" s="1">
-        <v>5</v>
+      <c r="B89" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>82</v>
@@ -3259,8 +3345,8 @@
       <c r="A90" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B90" s="1">
-        <v>6</v>
+      <c r="B90" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>21</v>
@@ -3270,8 +3356,8 @@
       <c r="A91" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B91" s="1">
-        <v>888</v>
+      <c r="B91" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>23</v>
@@ -3281,8 +3367,8 @@
       <c r="A92" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B92" s="1">
-        <v>1</v>
+      <c r="B92" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>83</v>
@@ -3292,8 +3378,8 @@
       <c r="A93" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B93" s="1">
-        <v>2</v>
+      <c r="B93" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>84</v>
@@ -3303,8 +3389,8 @@
       <c r="A94" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B94" s="1">
-        <v>3</v>
+      <c r="B94" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>85</v>
@@ -3314,8 +3400,8 @@
       <c r="A95" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B95" s="1">
-        <v>4</v>
+      <c r="B95" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>86</v>
@@ -3325,8 +3411,8 @@
       <c r="A96" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B96" s="1">
-        <v>5</v>
+      <c r="B96" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>87</v>
@@ -3336,8 +3422,8 @@
       <c r="A97" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B97" s="1">
-        <v>6</v>
+      <c r="B97" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>88</v>
@@ -3347,8 +3433,8 @@
       <c r="A98" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B98" s="1">
-        <v>7</v>
+      <c r="B98" s="2" t="s">
+        <v>327</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>89</v>
@@ -3358,8 +3444,8 @@
       <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B99" s="1">
-        <v>8</v>
+      <c r="B99" s="2" t="s">
+        <v>328</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>90</v>
@@ -3369,8 +3455,8 @@
       <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B100" s="1">
-        <v>9</v>
+      <c r="B100" s="2" t="s">
+        <v>329</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>91</v>
@@ -3380,8 +3466,8 @@
       <c r="A101" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B101" s="1">
-        <v>10</v>
+      <c r="B101" s="2" t="s">
+        <v>330</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>92</v>
@@ -3391,8 +3477,8 @@
       <c r="A102" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B102" s="1">
-        <v>11</v>
+      <c r="B102" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>93</v>
@@ -3402,8 +3488,8 @@
       <c r="A103" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B103" s="1">
-        <v>12</v>
+      <c r="B103" s="2" t="s">
+        <v>332</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>94</v>
@@ -3413,8 +3499,8 @@
       <c r="A104" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B104" s="1">
-        <v>13</v>
+      <c r="B104" s="2" t="s">
+        <v>333</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>95</v>
@@ -3424,8 +3510,8 @@
       <c r="A105" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B105" s="1">
-        <v>14</v>
+      <c r="B105" s="2" t="s">
+        <v>334</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>96</v>
@@ -3435,8 +3521,8 @@
       <c r="A106" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B106" s="1">
-        <v>15</v>
+      <c r="B106" s="2" t="s">
+        <v>335</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>21</v>
@@ -3446,8 +3532,8 @@
       <c r="A107" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B107" s="1">
-        <v>16</v>
+      <c r="B107" s="2" t="s">
+        <v>336</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>97</v>
@@ -3457,8 +3543,8 @@
       <c r="A108" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B108" s="1">
-        <v>888</v>
+      <c r="B108" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>23</v>
@@ -3468,8 +3554,8 @@
       <c r="A109" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B109" s="1">
-        <v>1</v>
+      <c r="B109" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>99</v>
@@ -3479,8 +3565,8 @@
       <c r="A110" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B110" s="1">
-        <v>2</v>
+      <c r="B110" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>100</v>
@@ -3490,8 +3576,8 @@
       <c r="A111" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B111" s="1">
-        <v>3</v>
+      <c r="B111" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>101</v>
@@ -3501,8 +3587,8 @@
       <c r="A112" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B112" s="1">
-        <v>4</v>
+      <c r="B112" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>102</v>
@@ -3512,8 +3598,8 @@
       <c r="A113" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B113" s="1">
-        <v>5</v>
+      <c r="B113" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>103</v>
@@ -3523,8 +3609,8 @@
       <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B114" s="1">
-        <v>6</v>
+      <c r="B114" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>104</v>
@@ -3534,8 +3620,8 @@
       <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B115" s="1">
-        <v>7</v>
+      <c r="B115" s="2" t="s">
+        <v>327</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>105</v>
@@ -3545,8 +3631,8 @@
       <c r="A116" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B116" s="1">
-        <v>8</v>
+      <c r="B116" s="2" t="s">
+        <v>328</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>106</v>
@@ -3556,8 +3642,8 @@
       <c r="A117" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B117" s="1">
-        <v>9</v>
+      <c r="B117" s="2" t="s">
+        <v>329</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>107</v>
@@ -3567,8 +3653,8 @@
       <c r="A118" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B118" s="1">
-        <v>10</v>
+      <c r="B118" s="2" t="s">
+        <v>330</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>108</v>
@@ -3578,8 +3664,8 @@
       <c r="A119" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B119" s="1">
-        <v>11</v>
+      <c r="B119" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>109</v>
@@ -3589,8 +3675,8 @@
       <c r="A120" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B120" s="1">
-        <v>12</v>
+      <c r="B120" s="2" t="s">
+        <v>332</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>110</v>
@@ -3600,8 +3686,8 @@
       <c r="A121" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B121" s="1">
-        <v>13</v>
+      <c r="B121" s="2" t="s">
+        <v>333</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>111</v>
@@ -3611,8 +3697,8 @@
       <c r="A122" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B122" s="1">
-        <v>14</v>
+      <c r="B122" s="2" t="s">
+        <v>334</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>112</v>
@@ -3622,8 +3708,8 @@
       <c r="A123" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B123" s="1">
-        <v>15</v>
+      <c r="B123" s="2" t="s">
+        <v>335</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>21</v>
@@ -3633,8 +3719,8 @@
       <c r="A124" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B124" s="1">
-        <v>888</v>
+      <c r="B124" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>23</v>
@@ -3644,8 +3730,8 @@
       <c r="A125" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B125" s="1">
-        <v>1</v>
+      <c r="B125" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>78</v>
@@ -3655,8 +3741,8 @@
       <c r="A126" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B126" s="1">
-        <v>2</v>
+      <c r="B126" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>79</v>
@@ -3666,8 +3752,8 @@
       <c r="A127" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B127" s="1">
-        <v>3</v>
+      <c r="B127" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>80</v>
@@ -3677,8 +3763,8 @@
       <c r="A128" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B128" s="1">
-        <v>4</v>
+      <c r="B128" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>81</v>
@@ -3688,8 +3774,8 @@
       <c r="A129" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B129" s="1">
-        <v>5</v>
+      <c r="B129" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>82</v>
@@ -3699,8 +3785,8 @@
       <c r="A130" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B130" s="1">
-        <v>6</v>
+      <c r="B130" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>21</v>
@@ -3710,8 +3796,8 @@
       <c r="A131" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B131" s="1">
-        <v>888</v>
+      <c r="B131" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>23</v>
@@ -3721,8 +3807,8 @@
       <c r="A132" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B132" s="1">
-        <v>1</v>
+      <c r="B132" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>115</v>
@@ -3732,8 +3818,8 @@
       <c r="A133" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B133" s="1">
-        <v>0</v>
+      <c r="B133" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>116</v>
@@ -3743,8 +3829,8 @@
       <c r="A134" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B134" s="1">
-        <v>888</v>
+      <c r="B134" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>23</v>
@@ -3754,8 +3840,8 @@
       <c r="A135" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B135" s="1">
-        <v>999</v>
+      <c r="B135" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>22</v>
@@ -3765,8 +3851,8 @@
       <c r="A136" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B136" s="1">
-        <v>0</v>
+      <c r="B136" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>118</v>
@@ -3776,8 +3862,8 @@
       <c r="A137" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B137" s="1">
-        <v>1</v>
+      <c r="B137" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>119</v>
@@ -3787,8 +3873,8 @@
       <c r="A138" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B138" s="1">
-        <v>2</v>
+      <c r="B138" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>120</v>
@@ -3798,8 +3884,8 @@
       <c r="A139" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B139" s="2">
-        <v>888</v>
+      <c r="B139" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>23</v>
@@ -3809,8 +3895,8 @@
       <c r="A140" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B140" s="2">
-        <v>0</v>
+      <c r="B140" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>122</v>
@@ -3820,8 +3906,8 @@
       <c r="A141" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B141" s="2">
-        <v>1</v>
+      <c r="B141" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>83</v>
@@ -3831,8 +3917,8 @@
       <c r="A142" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B142" s="2">
-        <v>2</v>
+      <c r="B142" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>84</v>
@@ -3842,8 +3928,8 @@
       <c r="A143" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B143" s="2">
-        <v>3</v>
+      <c r="B143" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>85</v>
@@ -3853,8 +3939,8 @@
       <c r="A144" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B144" s="2">
-        <v>4</v>
+      <c r="B144" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>86</v>
@@ -3864,8 +3950,8 @@
       <c r="A145" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B145" s="2">
-        <v>5</v>
+      <c r="B145" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>87</v>
@@ -3875,8 +3961,8 @@
       <c r="A146" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B146" s="2">
-        <v>6</v>
+      <c r="B146" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>88</v>
@@ -3886,8 +3972,8 @@
       <c r="A147" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B147" s="2">
-        <v>7</v>
+      <c r="B147" s="2" t="s">
+        <v>327</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>89</v>
@@ -3897,8 +3983,8 @@
       <c r="A148" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B148" s="2">
-        <v>8</v>
+      <c r="B148" s="2" t="s">
+        <v>328</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>90</v>
@@ -3908,8 +3994,8 @@
       <c r="A149" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B149" s="2">
-        <v>9</v>
+      <c r="B149" s="2" t="s">
+        <v>329</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>91</v>
@@ -3919,8 +4005,8 @@
       <c r="A150" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B150" s="2">
-        <v>10</v>
+      <c r="B150" s="2" t="s">
+        <v>330</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>92</v>
@@ -3930,8 +4016,8 @@
       <c r="A151" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B151" s="2">
-        <v>11</v>
+      <c r="B151" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>93</v>
@@ -3941,8 +4027,8 @@
       <c r="A152" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B152" s="2">
-        <v>12</v>
+      <c r="B152" s="2" t="s">
+        <v>332</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>94</v>
@@ -3952,8 +4038,8 @@
       <c r="A153" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B153" s="2">
-        <v>13</v>
+      <c r="B153" s="2" t="s">
+        <v>333</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>95</v>
@@ -3963,8 +4049,8 @@
       <c r="A154" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B154" s="2">
-        <v>14</v>
+      <c r="B154" s="2" t="s">
+        <v>334</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>21</v>
@@ -3974,8 +4060,8 @@
       <c r="A155" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B155" s="2">
-        <v>888</v>
+      <c r="B155" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>23</v>
@@ -3985,8 +4071,8 @@
       <c r="A156" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B156" s="2">
-        <v>4</v>
+      <c r="B156" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>125</v>
@@ -3996,8 +4082,8 @@
       <c r="A157" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B157" s="2">
-        <v>3</v>
+      <c r="B157" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>126</v>
@@ -4007,8 +4093,8 @@
       <c r="A158" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B158" s="2">
-        <v>2</v>
+      <c r="B158" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>127</v>
@@ -4018,8 +4104,8 @@
       <c r="A159" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B159" s="2">
-        <v>1</v>
+      <c r="B159" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>128</v>
@@ -4029,8 +4115,8 @@
       <c r="A160" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B160" s="2">
-        <v>0</v>
+      <c r="B160" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>118</v>
@@ -4040,8 +4126,8 @@
       <c r="A161" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B161" s="2">
-        <v>888</v>
+      <c r="B161" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>23</v>
@@ -4051,8 +4137,8 @@
       <c r="A162" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B162" s="2">
-        <v>1</v>
+      <c r="B162" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>130</v>
@@ -4062,8 +4148,8 @@
       <c r="A163" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B163" s="2">
-        <v>2</v>
+      <c r="B163" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>131</v>
@@ -4073,8 +4159,8 @@
       <c r="A164" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B164" s="2">
-        <v>3</v>
+      <c r="B164" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>132</v>
@@ -4084,8 +4170,8 @@
       <c r="A165" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B165" s="2">
-        <v>4</v>
+      <c r="B165" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>133</v>
@@ -4095,8 +4181,8 @@
       <c r="A166" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B166" s="2">
-        <v>5</v>
+      <c r="B166" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>134</v>
@@ -4106,8 +4192,8 @@
       <c r="A167" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B167" s="2">
-        <v>6</v>
+      <c r="B167" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>21</v>
@@ -4117,8 +4203,8 @@
       <c r="A168" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B168" s="2">
-        <v>888</v>
+      <c r="B168" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>23</v>
@@ -4128,8 +4214,8 @@
       <c r="A169" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B169" s="2">
-        <v>999</v>
+      <c r="B169" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>22</v>
@@ -4139,8 +4225,8 @@
       <c r="A170" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B170" s="2">
-        <v>0</v>
+      <c r="B170" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>136</v>
@@ -4150,8 +4236,8 @@
       <c r="A171" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B171" s="2">
-        <v>1</v>
+      <c r="B171" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>137</v>
@@ -4161,8 +4247,8 @@
       <c r="A172" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B172" s="2">
-        <v>888</v>
+      <c r="B172" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>23</v>
@@ -4172,8 +4258,8 @@
       <c r="A173" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B173" s="2">
-        <v>1</v>
+      <c r="B173" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>20</v>
@@ -4183,8 +4269,8 @@
       <c r="A174" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B174" s="2">
-        <v>0</v>
+      <c r="B174" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>19</v>
@@ -4194,8 +4280,8 @@
       <c r="A175" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B175" s="2">
-        <v>2</v>
+      <c r="B175" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>139</v>
@@ -4205,8 +4291,8 @@
       <c r="A176" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B176" s="2">
-        <v>888</v>
+      <c r="B176" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>23</v>
@@ -4216,8 +4302,8 @@
       <c r="A177" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B177" s="2">
-        <v>1</v>
+      <c r="B177" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>141</v>
@@ -4227,8 +4313,8 @@
       <c r="A178" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B178" s="2">
-        <v>2</v>
+      <c r="B178" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C178" s="2" t="s">
         <v>142</v>
@@ -4238,8 +4324,8 @@
       <c r="A179" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B179" s="2">
-        <v>3</v>
+      <c r="B179" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>143</v>
@@ -4249,8 +4335,8 @@
       <c r="A180" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B180" s="2">
-        <v>0</v>
+      <c r="B180" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>16</v>
@@ -4260,8 +4346,8 @@
       <c r="A181" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B181" s="2">
-        <v>888</v>
+      <c r="B181" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>23</v>
@@ -4271,8 +4357,8 @@
       <c r="A182" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B182" s="2">
-        <v>999</v>
+      <c r="B182" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>22</v>
@@ -4282,8 +4368,8 @@
       <c r="A183" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B183" s="2">
-        <v>0</v>
+      <c r="B183" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>146</v>
@@ -4293,8 +4379,8 @@
       <c r="A184" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B184" s="2">
-        <v>1</v>
+      <c r="B184" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>147</v>
@@ -4304,8 +4390,8 @@
       <c r="A185" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B185" s="2">
-        <v>2</v>
+      <c r="B185" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>148</v>
@@ -4315,8 +4401,8 @@
       <c r="A186" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B186" s="2">
-        <v>3</v>
+      <c r="B186" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>149</v>
@@ -4326,8 +4412,8 @@
       <c r="A187" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B187" s="2">
-        <v>4</v>
+      <c r="B187" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>21</v>
@@ -4337,8 +4423,8 @@
       <c r="A188" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B188" s="2">
-        <v>888</v>
+      <c r="B188" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>23</v>
@@ -4348,8 +4434,8 @@
       <c r="A189" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B189" s="2">
-        <v>1</v>
+      <c r="B189" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>150</v>
@@ -4359,8 +4445,8 @@
       <c r="A190" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B190" s="2">
-        <v>2</v>
+      <c r="B190" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C190" s="2" t="s">
         <v>151</v>
@@ -4370,8 +4456,8 @@
       <c r="A191" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B191" s="2">
-        <v>3</v>
+      <c r="B191" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>152</v>
@@ -4381,8 +4467,8 @@
       <c r="A192" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B192" s="2">
-        <v>4</v>
+      <c r="B192" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>153</v>
@@ -4392,8 +4478,8 @@
       <c r="A193" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B193" s="2">
-        <v>5</v>
+      <c r="B193" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>154</v>
@@ -4403,8 +4489,8 @@
       <c r="A194" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B194" s="2">
-        <v>888</v>
+      <c r="B194" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C194" s="2" t="s">
         <v>23</v>
@@ -4414,8 +4500,8 @@
       <c r="A195" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B195" s="2">
-        <v>999</v>
+      <c r="B195" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C195" s="2" t="s">
         <v>22</v>
@@ -4425,8 +4511,8 @@
       <c r="A196" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B196" s="2">
-        <v>0</v>
+      <c r="B196" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C196" s="2" t="s">
         <v>146</v>
@@ -4436,8 +4522,8 @@
       <c r="A197" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B197" s="2">
-        <v>1</v>
+      <c r="B197" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>156</v>
@@ -4447,8 +4533,8 @@
       <c r="A198" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B198" s="2">
-        <v>2</v>
+      <c r="B198" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>157</v>
@@ -4458,8 +4544,8 @@
       <c r="A199" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B199" s="2">
-        <v>888</v>
+      <c r="B199" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>23</v>
@@ -4469,8 +4555,8 @@
       <c r="A200" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B200" s="2">
-        <v>999</v>
+      <c r="B200" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>22</v>
@@ -4480,8 +4566,8 @@
       <c r="A201" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B201" s="2">
-        <v>1</v>
+      <c r="B201" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>29</v>
@@ -4491,8 +4577,8 @@
       <c r="A202" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B202" s="2">
-        <v>0</v>
+      <c r="B202" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>30</v>
@@ -4502,8 +4588,8 @@
       <c r="A203" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B203" s="2">
-        <v>1</v>
+      <c r="B203" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C203" s="2" t="s">
         <v>29</v>
@@ -4513,8 +4599,8 @@
       <c r="A204" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B204" s="2">
-        <v>0</v>
+      <c r="B204" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>30</v>
@@ -4524,8 +4610,8 @@
       <c r="A205" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B205" s="2">
-        <v>2</v>
+      <c r="B205" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>160</v>
@@ -4535,8 +4621,8 @@
       <c r="A206" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B206" s="2">
-        <v>1</v>
+      <c r="B206" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>15</v>
@@ -4546,8 +4632,8 @@
       <c r="A207" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B207" s="2">
-        <v>0</v>
+      <c r="B207" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C207" s="2" t="s">
         <v>16</v>
@@ -4557,8 +4643,8 @@
       <c r="A208" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B208" s="2">
-        <v>3</v>
+      <c r="B208" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>163</v>
@@ -4568,8 +4654,8 @@
       <c r="A209" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B209" s="2">
-        <v>4</v>
+      <c r="B209" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C209" s="2" t="s">
         <v>175</v>
@@ -4579,8 +4665,8 @@
       <c r="A210" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B210" s="2">
-        <v>1</v>
+      <c r="B210" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>174</v>
@@ -4590,8 +4676,8 @@
       <c r="A211" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B211" s="2">
-        <v>1</v>
+      <c r="B211" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C211" s="2" t="s">
         <v>194</v>
@@ -4601,8 +4687,8 @@
       <c r="A212" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B212" s="2">
-        <v>888</v>
+      <c r="B212" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>23</v>
@@ -4612,8 +4698,8 @@
       <c r="A213" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B213" s="2">
-        <v>0</v>
+      <c r="B213" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>19</v>
@@ -4623,8 +4709,8 @@
       <c r="A214" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B214" s="2">
-        <v>1</v>
+      <c r="B214" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C214" s="2" t="s">
         <v>20</v>
@@ -4634,8 +4720,8 @@
       <c r="A215" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B215" s="1">
-        <v>1</v>
+      <c r="B215" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>304</v>
@@ -4645,8 +4731,8 @@
       <c r="A216" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B216" s="1">
-        <v>2</v>
+      <c r="B216" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>305</v>
@@ -4656,8 +4742,8 @@
       <c r="A217" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B217" s="1">
-        <v>3</v>
+      <c r="B217" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>306</v>
@@ -4667,8 +4753,8 @@
       <c r="A218" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B218" s="1">
-        <v>4</v>
+      <c r="B218" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>307</v>
@@ -4678,8 +4764,8 @@
       <c r="A219" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B219" s="1">
-        <v>5</v>
+      <c r="B219" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>308</v>
@@ -4689,8 +4775,8 @@
       <c r="A220" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B220" s="1">
-        <v>6</v>
+      <c r="B220" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>309</v>
@@ -4700,8 +4786,8 @@
       <c r="A221" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B221" s="1">
-        <v>7</v>
+      <c r="B221" s="2" t="s">
+        <v>327</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>310</v>
@@ -4711,8 +4797,8 @@
       <c r="A222" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B222" s="1">
-        <v>8</v>
+      <c r="B222" s="2" t="s">
+        <v>328</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>21</v>
@@ -4722,8 +4808,8 @@
       <c r="A223" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B223" s="1">
-        <v>9</v>
+      <c r="B223" s="2" t="s">
+        <v>329</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>311</v>
@@ -4733,8 +4819,8 @@
       <c r="A224" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B224" s="1">
-        <v>888</v>
+      <c r="B224" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>23</v>
@@ -4744,8 +4830,8 @@
       <c r="A225" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B225" s="1">
-        <v>0</v>
+      <c r="B225" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>122</v>
@@ -4755,8 +4841,8 @@
       <c r="A226" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B226" s="1">
-        <v>1</v>
+      <c r="B226" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>312</v>
@@ -4766,8 +4852,8 @@
       <c r="A227" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B227" s="1">
-        <v>2</v>
+      <c r="B227" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>313</v>
@@ -4777,8 +4863,8 @@
       <c r="A228" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B228" s="1">
-        <v>3</v>
+      <c r="B228" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>314</v>
@@ -4788,8 +4874,8 @@
       <c r="A229" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B229" s="1">
-        <v>4</v>
+      <c r="B229" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>315</v>
@@ -4799,8 +4885,8 @@
       <c r="A230" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B230" s="1">
-        <v>5</v>
+      <c r="B230" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>21</v>
@@ -4810,8 +4896,8 @@
       <c r="A231" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B231" s="1">
-        <v>888</v>
+      <c r="B231" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>23</v>

</xml_diff>